<commit_message>
Added a my part of the tutorial and journal.
</commit_message>
<xml_diff>
--- a/topics/01_arduino/Arduino_IR_Chat_LCD/Journal.xlsx
+++ b/topics/01_arduino/Arduino_IR_Chat_LCD/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Github\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235CEC4C-D658-451B-8409-A9C21A20BB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D17D70-3DB5-45E0-A42D-06B41E047380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t xml:space="preserve">Date	</t>
   </si>
@@ -89,13 +89,40 @@
   </si>
   <si>
     <t>Number of worked hours</t>
+  </si>
+  <si>
+    <t>11.11.2022</t>
+  </si>
+  <si>
+    <t>Discussed what final project we could do and looked online for the materials.</t>
+  </si>
+  <si>
+    <t>Discussed what final project we could do and looked online for the materials</t>
+  </si>
+  <si>
+    <t>15.11.2022</t>
+  </si>
+  <si>
+    <t>Worked on the tutorial</t>
+  </si>
+  <si>
+    <t>16.11.2023</t>
+  </si>
+  <si>
+    <t>16.11.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandro </t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +253,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -929,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,7 +1113,7 @@
         <v>20</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1094,7 +1127,7 @@
         <v>20</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1108,7 +1141,7 @@
         <v>18</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1122,10 +1155,81 @@
         <v>19</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>